<commit_message>
Made changes to compute speed, power, COT for single hop
</commit_message>
<xml_diff>
--- a/ms4_part2_data.xlsx
+++ b/ms4_part2_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\77bis\Desktop\ECE489_M4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo Song\Desktop\ECE489_M4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E4F366-4640-49FA-AED1-45C2ABFFDC5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FA043A-040E-40C8-8946-F3A13938445B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{FCEC43C9-A48B-4AF8-B341-B11679AC7D90}"/>
+    <workbookView xWindow="7665" yWindow="3330" windowWidth="21600" windowHeight="11385" xr2:uid="{FCEC43C9-A48B-4AF8-B341-B11679AC7D90}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -414,20 +412,20 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -441,7 +439,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -449,30 +447,30 @@
         <v>-8.6300000000000002E-2</v>
       </c>
       <c r="C2">
-        <v>-0.40460000000000002</v>
+        <v>-0.32119999999999999</v>
       </c>
       <c r="D2">
         <v>117.5939</v>
       </c>
       <c r="E2">
-        <v>64.264200000000002</v>
+        <v>42.278399999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.64949999999999997</v>
+        <v>0.71</v>
       </c>
       <c r="C3">
-        <v>1.0928</v>
+        <v>1.0570999999999999</v>
       </c>
       <c r="D3">
-        <v>82.196299999999994</v>
+        <v>109.5784</v>
       </c>
       <c r="E3">
-        <v>6.1761999999999997</v>
+        <v>5.0027999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>